<commit_message>
Modif dictionnaire des données - Ajout champ offre_salaire
</commit_message>
<xml_diff>
--- a/TRAVAIL/Documentation/Dictionnaire des données AmdWeb.xlsx
+++ b/TRAVAIL/Documentation/Dictionnaire des données AmdWeb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cciraformation-my.sharepoint.com/personal/jonathan_legrand_ccicampus_fr/Documents/Phase 2/Dossier d'analyse AmdWeb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\AmdWeb_Projet_2\TRAVAIL\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="501" documentId="8_{87301D57-2068-4F66-8B72-2489156D98D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAEB78D4-17C6-4CCB-9D88-7B3FDD3AF106}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC48160-060A-47C3-A957-473012777F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15990" xr2:uid="{C2CF0808-BAC5-4DD3-8137-2CDC69554DDC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2CF0808-BAC5-4DD3-8137-2CDC69554DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>tc={B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}</author>
   </authors>
   <commentList>
-    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
+    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="101">
   <si>
     <t>Dictionnaire des données</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>Nom de la ville</t>
+  </si>
+  <si>
+    <t>offre_salaire</t>
+  </si>
+  <si>
+    <t>Salaire de l'offre</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +433,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -630,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -755,6 +767,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,19 +809,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1117,7 +1141,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E28" dT="2023-01-18T12:49:56.50" personId="{0BD7DE6D-B856-4F05-9EC3-BE2BB041533E}" id="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
+  <threadedComment ref="E29" dT="2023-01-18T12:49:56.50" personId="{0BD7DE6D-B856-4F05-9EC3-BE2BB041533E}" id="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
     <text>ADMINISTRATEUR
 MODERATEUR
 CANDIDAT
@@ -1129,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E3A71C-C73C-46AB-9D56-E27F7E7430A4}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,14 +1172,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1178,7 +1202,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="33" t="s">
@@ -1198,7 +1222,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="34" t="s">
         <v>12</v>
       </c>
@@ -1214,7 +1238,7 @@
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="35" t="s">
         <v>15</v>
       </c>
@@ -1232,7 +1256,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="34" t="s">
         <v>18</v>
       </c>
@@ -1248,7 +1272,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="35" t="s">
         <v>21</v>
       </c>
@@ -1264,7 +1288,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="34" t="s">
         <v>23</v>
       </c>
@@ -1282,7 +1306,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="35" t="s">
         <v>25</v>
       </c>
@@ -1298,7 +1322,7 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="34" t="s">
         <v>27</v>
       </c>
@@ -1314,7 +1338,7 @@
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="36" t="s">
         <v>29</v>
       </c>
@@ -1328,7 +1352,7 @@
       <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="37" t="s">
         <v>32</v>
       </c>
@@ -1344,7 +1368,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="35" t="s">
         <v>34</v>
       </c>
@@ -1360,7 +1384,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="34" t="s">
         <v>36</v>
       </c>
@@ -1378,7 +1402,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="38" t="s">
         <v>39</v>
       </c>
@@ -1396,7 +1420,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="52" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="39" t="s">
@@ -1416,7 +1440,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="35" t="s">
         <v>45</v>
       </c>
@@ -1430,7 +1454,7 @@
       <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="34" t="s">
         <v>47</v>
       </c>
@@ -1446,23 +1470,23 @@
       <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
-      <c r="B19" s="52" t="s">
+      <c r="A19" s="53"/>
+      <c r="B19" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="53" t="s">
+      <c r="D19" s="45"/>
+      <c r="E19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="34" t="s">
         <v>51</v>
       </c>
@@ -1480,21 +1504,21 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="52" t="s">
+      <c r="A21" s="53"/>
+      <c r="B21" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="53" t="s">
+      <c r="D21" s="45"/>
+      <c r="E21" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="55"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="34" t="s">
         <v>56</v>
       </c>
@@ -1509,378 +1533,394 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
-      <c r="B23" s="52" t="s">
+    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="53"/>
+      <c r="B23" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="58">
+        <v>7</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="59"/>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53"/>
+      <c r="B24" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C24" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="54">
-        <v>11</v>
-      </c>
-      <c r="E23" s="53" t="s">
+      <c r="D24" s="45">
+        <v>11</v>
+      </c>
+      <c r="E24" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="55" t="s">
+      <c r="F24" s="46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="49"/>
-      <c r="B24" s="40" t="s">
+    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="54"/>
+      <c r="B25" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="31">
-        <v>11</v>
-      </c>
-      <c r="E24" s="12" t="s">
+      <c r="D25" s="31">
+        <v>11</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F25" s="32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B26" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C26" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="54">
-        <v>11</v>
-      </c>
-      <c r="E25" s="53" t="s">
+      <c r="D26" s="45">
+        <v>11</v>
+      </c>
+      <c r="E26" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
-      <c r="B26" s="34" t="s">
+      <c r="F26" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="51"/>
+      <c r="B27" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D27" s="14">
         <v>255</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="46"/>
-      <c r="B27" s="52" t="s">
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="51"/>
+      <c r="B28" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C28" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="54">
-        <v>11</v>
-      </c>
-      <c r="E27" s="53" t="s">
+      <c r="D28" s="45">
+        <v>11</v>
+      </c>
+      <c r="E28" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="55" t="s">
+      <c r="F28" s="46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
+    <row r="29" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B29" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="10">
-        <v>11</v>
-      </c>
-      <c r="E28" s="9" t="s">
+      <c r="D29" s="10">
+        <v>11</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="44"/>
-    </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="49"/>
-      <c r="B29" s="52" t="s">
+      <c r="F29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="49"/>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="54"/>
+      <c r="B30" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C30" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="54">
+      <c r="D30" s="45">
         <v>20</v>
       </c>
-      <c r="E29" s="53" t="s">
+      <c r="E30" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="55"/>
-      <c r="G29" s="44"/>
-    </row>
-    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
+      <c r="F30" s="46"/>
+      <c r="G30" s="49"/>
+    </row>
+    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B31" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="10">
-        <v>11</v>
-      </c>
-      <c r="E30" s="9" t="s">
+      <c r="D31" s="10">
+        <v>11</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F30" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
-      <c r="B31" s="52" t="s">
+      <c r="F31" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="51"/>
+      <c r="B32" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="53" t="s">
+      <c r="C32" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D32" s="45">
         <v>255</v>
       </c>
-      <c r="E31" s="53" t="s">
+      <c r="E32" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="55"/>
-    </row>
-    <row r="32" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="46"/>
-      <c r="B32" s="40" t="s">
+      <c r="F32" s="46"/>
+    </row>
+    <row r="33" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="51"/>
+      <c r="B33" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C33" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="31">
-        <v>11</v>
-      </c>
-      <c r="E32" s="12" t="s">
+      <c r="D33" s="31">
+        <v>11</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="51" t="s">
+      <c r="F33" s="42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B34" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="53" t="s">
+      <c r="C34" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="54">
-        <v>11</v>
-      </c>
-      <c r="E33" s="53" t="s">
+      <c r="D34" s="45">
+        <v>11</v>
+      </c>
+      <c r="E34" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48"/>
-      <c r="B34" s="34" t="s">
+      <c r="F34" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="53"/>
+      <c r="B35" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="14">
-        <v>11</v>
-      </c>
-      <c r="E34" s="11" t="s">
+      <c r="D35" s="14">
+        <v>11</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F35" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="49"/>
-      <c r="B35" s="52" t="s">
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="54"/>
+      <c r="B36" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="53" t="s">
+      <c r="C36" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="54">
-        <v>11</v>
-      </c>
-      <c r="E35" s="53" t="s">
+      <c r="D36" s="45">
+        <v>11</v>
+      </c>
+      <c r="E36" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="55" t="s">
+      <c r="F36" s="46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B37" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="10">
-        <v>11</v>
-      </c>
-      <c r="E36" s="9" t="s">
+      <c r="D37" s="10">
+        <v>11</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
-      <c r="B37" s="52" t="s">
+      <c r="F37" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="51"/>
+      <c r="B38" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="53" t="s">
+      <c r="C38" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="53" t="s">
+      <c r="D38" s="45"/>
+      <c r="E38" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="55"/>
-    </row>
-    <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
-      <c r="B38" s="34" t="s">
+      <c r="F38" s="46"/>
+    </row>
+    <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="51"/>
+      <c r="B39" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="14">
-        <v>11</v>
-      </c>
-      <c r="E38" s="11" t="s">
+      <c r="D39" s="14">
+        <v>11</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F39" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
-      <c r="B39" s="52" t="s">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="51"/>
+      <c r="B40" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="53" t="s">
+      <c r="C40" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="54">
-        <v>11</v>
-      </c>
-      <c r="E39" s="53" t="s">
+      <c r="D40" s="45">
+        <v>11</v>
+      </c>
+      <c r="E40" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="55" t="s">
+      <c r="F40" s="46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B41" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="10">
-        <v>11</v>
-      </c>
-      <c r="E40" s="9" t="s">
+      <c r="D41" s="10">
+        <v>11</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="48"/>
-      <c r="B41" s="52" t="s">
+      <c r="F41" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="53"/>
+      <c r="B42" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="53" t="s">
+      <c r="C42" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="54">
+      <c r="D42" s="45">
         <v>5</v>
       </c>
-      <c r="E41" s="53" t="s">
+      <c r="E42" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="55"/>
-    </row>
-    <row r="42" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="49"/>
-      <c r="B42" s="40" t="s">
+      <c r="F42" s="46"/>
+    </row>
+    <row r="43" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="54"/>
+      <c r="B43" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="31">
+      <c r="D43" s="31">
         <v>255</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E43" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F42" s="32"/>
+      <c r="F43" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A43"/>
     <mergeCell ref="A3:A15"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
mcv et smarty adaptation
</commit_message>
<xml_diff>
--- a/TRAVAIL/Documentation/Dictionnaire des données AmdWeb.xlsx
+++ b/TRAVAIL/Documentation/Dictionnaire des données AmdWeb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cciraformation-my.sharepoint.com/personal/jonathan_legrand_ccicampus_fr/Documents/Phase 2/Dossier d'analyse AmdWeb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\AmdWeb_Projet_2\TRAVAIL\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="501" documentId="8_{87301D57-2068-4F66-8B72-2489156D98D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAEB78D4-17C6-4CCB-9D88-7B3FDD3AF106}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC48160-060A-47C3-A957-473012777F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15990" xr2:uid="{C2CF0808-BAC5-4DD3-8137-2CDC69554DDC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C2CF0808-BAC5-4DD3-8137-2CDC69554DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>tc={B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}</author>
   </authors>
   <commentList>
-    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
+    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="101">
   <si>
     <t>Dictionnaire des données</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>Nom de la ville</t>
+  </si>
+  <si>
+    <t>offre_salaire</t>
+  </si>
+  <si>
+    <t>Salaire de l'offre</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +433,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -630,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -755,6 +767,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,19 +809,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1117,7 +1141,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E28" dT="2023-01-18T12:49:56.50" personId="{0BD7DE6D-B856-4F05-9EC3-BE2BB041533E}" id="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
+  <threadedComment ref="E29" dT="2023-01-18T12:49:56.50" personId="{0BD7DE6D-B856-4F05-9EC3-BE2BB041533E}" id="{B70413EB-A7E6-48C2-96F9-DF9E77E0B56E}">
     <text>ADMINISTRATEUR
 MODERATEUR
 CANDIDAT
@@ -1129,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E3A71C-C73C-46AB-9D56-E27F7E7430A4}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,14 +1172,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1178,7 +1202,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="33" t="s">
@@ -1198,7 +1222,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="34" t="s">
         <v>12</v>
       </c>
@@ -1214,7 +1238,7 @@
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="35" t="s">
         <v>15</v>
       </c>
@@ -1232,7 +1256,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="34" t="s">
         <v>18</v>
       </c>
@@ -1248,7 +1272,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="35" t="s">
         <v>21</v>
       </c>
@@ -1264,7 +1288,7 @@
       <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="34" t="s">
         <v>23</v>
       </c>
@@ -1282,7 +1306,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="35" t="s">
         <v>25</v>
       </c>
@@ -1298,7 +1322,7 @@
       <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="34" t="s">
         <v>27</v>
       </c>
@@ -1314,7 +1338,7 @@
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="36" t="s">
         <v>29</v>
       </c>
@@ -1328,7 +1352,7 @@
       <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="37" t="s">
         <v>32</v>
       </c>
@@ -1344,7 +1368,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="35" t="s">
         <v>34</v>
       </c>
@@ -1360,7 +1384,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="34" t="s">
         <v>36</v>
       </c>
@@ -1378,7 +1402,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="38" t="s">
         <v>39</v>
       </c>
@@ -1396,7 +1420,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="52" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="39" t="s">
@@ -1416,7 +1440,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="35" t="s">
         <v>45</v>
       </c>
@@ -1430,7 +1454,7 @@
       <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="34" t="s">
         <v>47</v>
       </c>
@@ -1446,23 +1470,23 @@
       <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
-      <c r="B19" s="52" t="s">
+      <c r="A19" s="53"/>
+      <c r="B19" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="54"/>
-      <c r="E19" s="53" t="s">
+      <c r="D19" s="45"/>
+      <c r="E19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="46" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="34" t="s">
         <v>51</v>
       </c>
@@ -1480,21 +1504,21 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="52" t="s">
+      <c r="A21" s="53"/>
+      <c r="B21" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="53" t="s">
+      <c r="D21" s="45"/>
+      <c r="E21" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="55"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="34" t="s">
         <v>56</v>
       </c>
@@ -1509,378 +1533,394 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
-      <c r="B23" s="52" t="s">
+    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="53"/>
+      <c r="B23" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="58">
+        <v>7</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="59"/>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53"/>
+      <c r="B24" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C24" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="54">
-        <v>11</v>
-      </c>
-      <c r="E23" s="53" t="s">
+      <c r="D24" s="45">
+        <v>11</v>
+      </c>
+      <c r="E24" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="55" t="s">
+      <c r="F24" s="46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="49"/>
-      <c r="B24" s="40" t="s">
+    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="54"/>
+      <c r="B25" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="31">
-        <v>11</v>
-      </c>
-      <c r="E24" s="12" t="s">
+      <c r="D25" s="31">
+        <v>11</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F25" s="32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+    <row r="26" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B26" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C26" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="54">
-        <v>11</v>
-      </c>
-      <c r="E25" s="53" t="s">
+      <c r="D26" s="45">
+        <v>11</v>
+      </c>
+      <c r="E26" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
-      <c r="B26" s="34" t="s">
+      <c r="F26" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="51"/>
+      <c r="B27" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D27" s="14">
         <v>255</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="46"/>
-      <c r="B27" s="52" t="s">
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="51"/>
+      <c r="B28" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C28" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="54">
-        <v>11</v>
-      </c>
-      <c r="E27" s="53" t="s">
+      <c r="D28" s="45">
+        <v>11</v>
+      </c>
+      <c r="E28" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="55" t="s">
+      <c r="F28" s="46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
+    <row r="29" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B29" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="10">
-        <v>11</v>
-      </c>
-      <c r="E28" s="9" t="s">
+      <c r="D29" s="10">
+        <v>11</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="44"/>
-    </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="49"/>
-      <c r="B29" s="52" t="s">
+      <c r="F29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="49"/>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="54"/>
+      <c r="B30" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C30" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="54">
+      <c r="D30" s="45">
         <v>20</v>
       </c>
-      <c r="E29" s="53" t="s">
+      <c r="E30" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="55"/>
-      <c r="G29" s="44"/>
-    </row>
-    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
+      <c r="F30" s="46"/>
+      <c r="G30" s="49"/>
+    </row>
+    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B31" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="10">
-        <v>11</v>
-      </c>
-      <c r="E30" s="9" t="s">
+      <c r="D31" s="10">
+        <v>11</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F30" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
-      <c r="B31" s="52" t="s">
+      <c r="F31" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="51"/>
+      <c r="B32" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="53" t="s">
+      <c r="C32" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D32" s="45">
         <v>255</v>
       </c>
-      <c r="E31" s="53" t="s">
+      <c r="E32" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="55"/>
-    </row>
-    <row r="32" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="46"/>
-      <c r="B32" s="40" t="s">
+      <c r="F32" s="46"/>
+    </row>
+    <row r="33" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="51"/>
+      <c r="B33" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C33" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="31">
-        <v>11</v>
-      </c>
-      <c r="E32" s="12" t="s">
+      <c r="D33" s="31">
+        <v>11</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="51" t="s">
+      <c r="F33" s="42" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B34" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="53" t="s">
+      <c r="C34" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="54">
-        <v>11</v>
-      </c>
-      <c r="E33" s="53" t="s">
+      <c r="D34" s="45">
+        <v>11</v>
+      </c>
+      <c r="E34" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="48"/>
-      <c r="B34" s="34" t="s">
+      <c r="F34" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="53"/>
+      <c r="B35" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="14">
-        <v>11</v>
-      </c>
-      <c r="E34" s="11" t="s">
+      <c r="D35" s="14">
+        <v>11</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F35" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="49"/>
-      <c r="B35" s="52" t="s">
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="54"/>
+      <c r="B36" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="53" t="s">
+      <c r="C36" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="54">
-        <v>11</v>
-      </c>
-      <c r="E35" s="53" t="s">
+      <c r="D36" s="45">
+        <v>11</v>
+      </c>
+      <c r="E36" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="55" t="s">
+      <c r="F36" s="46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B37" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="10">
-        <v>11</v>
-      </c>
-      <c r="E36" s="9" t="s">
+      <c r="D37" s="10">
+        <v>11</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
-      <c r="B37" s="52" t="s">
+      <c r="F37" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="51"/>
+      <c r="B38" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="53" t="s">
+      <c r="C38" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="53" t="s">
+      <c r="D38" s="45"/>
+      <c r="E38" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="F37" s="55"/>
-    </row>
-    <row r="38" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
-      <c r="B38" s="34" t="s">
+      <c r="F38" s="46"/>
+    </row>
+    <row r="39" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="51"/>
+      <c r="B39" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="14">
-        <v>11</v>
-      </c>
-      <c r="E38" s="11" t="s">
+      <c r="D39" s="14">
+        <v>11</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F39" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
-      <c r="B39" s="52" t="s">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="51"/>
+      <c r="B40" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="53" t="s">
+      <c r="C40" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="54">
-        <v>11</v>
-      </c>
-      <c r="E39" s="53" t="s">
+      <c r="D40" s="45">
+        <v>11</v>
+      </c>
+      <c r="E40" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="55" t="s">
+      <c r="F40" s="46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B41" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="10">
-        <v>11</v>
-      </c>
-      <c r="E40" s="9" t="s">
+      <c r="D41" s="10">
+        <v>11</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="48"/>
-      <c r="B41" s="52" t="s">
+      <c r="F41" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="53"/>
+      <c r="B42" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="53" t="s">
+      <c r="C42" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="54">
+      <c r="D42" s="45">
         <v>5</v>
       </c>
-      <c r="E41" s="53" t="s">
+      <c r="E42" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="55"/>
-    </row>
-    <row r="42" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="49"/>
-      <c r="B42" s="40" t="s">
+      <c r="F42" s="46"/>
+    </row>
+    <row r="43" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="54"/>
+      <c r="B43" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="31">
+      <c r="D43" s="31">
         <v>255</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E43" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F42" s="32"/>
+      <c r="F43" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A43"/>
     <mergeCell ref="A3:A15"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>